<commit_message>
feat(phone): robust normalize/validate para aceitar 0+operadora (021), remover prefixos, adicionar 55 quando necessário e aceitar 8-15 dígitos
</commit_message>
<xml_diff>
--- a/public/lista de transissao whatsapp - 1 PREÇOS E COTACOES.xlsx
+++ b/public/lista de transissao whatsapp - 1 PREÇOS E COTACOES.xlsx
@@ -1,25 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBC6C8D4-4E0A-455B-AD53-F772FC5AC5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8180E197-359F-4A49-824D-B5C6F38391FA}"/>
+    <workbookView windowWidth="12075" windowHeight="6735"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -1079,25 +1070,368 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1105,24 +1439,310 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Moeda" xfId="2" builtinId="4"/>
+    <cellStyle name="Porcentagem" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Moeda [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Hyperlink seguido" xfId="7" builtinId="9"/>
+    <cellStyle name="Observação" xfId="8" builtinId="10"/>
+    <cellStyle name="Texto de Aviso" xfId="9" builtinId="11"/>
+    <cellStyle name="Título" xfId="10" builtinId="15"/>
+    <cellStyle name="Texto Explicativo" xfId="11" builtinId="53"/>
+    <cellStyle name="Título 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Título 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Título 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Título 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Entrada" xfId="16" builtinId="20"/>
+    <cellStyle name="Saída" xfId="17" builtinId="21"/>
+    <cellStyle name="Cálculo" xfId="18" builtinId="22"/>
+    <cellStyle name="Célula de Verificação" xfId="19" builtinId="23"/>
+    <cellStyle name="Célula Vinculada" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Bom" xfId="22" builtinId="26"/>
+    <cellStyle name="Ruim" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutro" xfId="24" builtinId="28"/>
+    <cellStyle name="Ênfase 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Ênfase 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Ênfase 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Ênfase 1" xfId="28" builtinId="32"/>
+    <cellStyle name="Ênfase 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Ênfase 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Ênfase 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Ênfase 2" xfId="32" builtinId="36"/>
+    <cellStyle name="Ênfase 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Ênfase 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Ênfase 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Ênfase 3" xfId="36" builtinId="40"/>
+    <cellStyle name="Ênfase 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Ênfase 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Ênfase 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Ênfase 4" xfId="40" builtinId="44"/>
+    <cellStyle name="Ênfase 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Ênfase 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Ênfase 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Ênfase 5" xfId="44" builtinId="48"/>
+    <cellStyle name="Ênfase 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Ênfase 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Ênfase 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Ênfase 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1171,7 +1791,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1204,26 +1824,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1256,23 +1859,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1434,1933 +2020,1410 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD89EFC7-0729-456D-8806-F4C4603A5E4F}">
-  <dimension ref="A1:C173"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A173"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="A163" sqref="A$1:A$1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
   <cols>
-    <col min="2" max="2" width="65.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="65.425" customWidth="1"/>
+    <col min="2" max="2" width="27.5666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>7</v>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>8</v>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>9</v>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>10</v>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>11</v>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>12</v>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>13</v>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>14</v>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>15</v>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>16</v>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>17</v>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>18</v>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>19</v>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>20</v>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>21</v>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>22</v>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>23</v>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>24</v>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>25</v>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>26</v>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>27</v>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>28</v>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>29</v>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>30</v>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>31</v>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>32</v>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
-      </c>
-      <c r="C32" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>33</v>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>34</v>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
-      </c>
-      <c r="C34" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>35</v>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>36</v>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>37</v>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
-      </c>
-      <c r="C37" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>38</v>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
-      </c>
-      <c r="C38" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>39</v>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>40</v>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
-      </c>
-      <c r="C40" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>41</v>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
-      </c>
-      <c r="C41" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>42</v>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>82</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
-      </c>
-      <c r="C42" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>43</v>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
-      </c>
-      <c r="C43" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>44</v>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>86</v>
-      </c>
-      <c r="C44" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>45</v>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>88</v>
       </c>
       <c r="B45" t="s">
-        <v>88</v>
-      </c>
-      <c r="C45" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>46</v>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>90</v>
       </c>
       <c r="B46" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>47</v>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>92</v>
       </c>
       <c r="B47" t="s">
-        <v>92</v>
-      </c>
-      <c r="C47" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>48</v>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>94</v>
       </c>
       <c r="B48" t="s">
-        <v>94</v>
-      </c>
-      <c r="C48" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>49</v>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>96</v>
       </c>
       <c r="B49" t="s">
-        <v>96</v>
-      </c>
-      <c r="C49" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>50</v>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>98</v>
       </c>
       <c r="B50" t="s">
-        <v>98</v>
-      </c>
-      <c r="C50" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>51</v>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>100</v>
       </c>
       <c r="B51" t="s">
-        <v>100</v>
-      </c>
-      <c r="C51" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>52</v>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>102</v>
       </c>
       <c r="B52" t="s">
-        <v>102</v>
-      </c>
-      <c r="C52" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>53</v>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>104</v>
       </c>
       <c r="B53" t="s">
-        <v>104</v>
-      </c>
-      <c r="C53" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>54</v>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>106</v>
       </c>
       <c r="B54" t="s">
-        <v>106</v>
-      </c>
-      <c r="C54" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>55</v>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>108</v>
       </c>
       <c r="B55" t="s">
-        <v>108</v>
-      </c>
-      <c r="C55" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>56</v>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>110</v>
       </c>
       <c r="B56" t="s">
-        <v>110</v>
-      </c>
-      <c r="C56" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>57</v>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>112</v>
       </c>
       <c r="B57" t="s">
-        <v>112</v>
-      </c>
-      <c r="C57" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>58</v>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>114</v>
       </c>
       <c r="B58" t="s">
-        <v>114</v>
-      </c>
-      <c r="C58" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>59</v>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>116</v>
       </c>
       <c r="B59" t="s">
-        <v>116</v>
-      </c>
-      <c r="C59" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>60</v>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>118</v>
       </c>
       <c r="B60" t="s">
-        <v>118</v>
-      </c>
-      <c r="C60" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>61</v>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>120</v>
       </c>
       <c r="B61" t="s">
-        <v>120</v>
-      </c>
-      <c r="C61" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>62</v>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>122</v>
       </c>
       <c r="B62" t="s">
-        <v>122</v>
-      </c>
-      <c r="C62" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>63</v>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>124</v>
       </c>
       <c r="B63" t="s">
-        <v>124</v>
-      </c>
-      <c r="C63" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>64</v>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>126</v>
       </c>
       <c r="B64" t="s">
-        <v>126</v>
-      </c>
-      <c r="C64" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>65</v>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>128</v>
       </c>
       <c r="B65" t="s">
-        <v>128</v>
-      </c>
-      <c r="C65" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>66</v>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>130</v>
       </c>
       <c r="B66" t="s">
-        <v>130</v>
-      </c>
-      <c r="C66" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>67</v>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>132</v>
       </c>
       <c r="B67" t="s">
-        <v>132</v>
-      </c>
-      <c r="C67" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>68</v>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>134</v>
       </c>
       <c r="B68" t="s">
-        <v>134</v>
-      </c>
-      <c r="C68" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>69</v>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>136</v>
       </c>
       <c r="B69" t="s">
-        <v>136</v>
-      </c>
-      <c r="C69" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>70</v>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>138</v>
       </c>
       <c r="B70" t="s">
-        <v>138</v>
-      </c>
-      <c r="C70" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>71</v>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>140</v>
       </c>
       <c r="B71" t="s">
-        <v>140</v>
-      </c>
-      <c r="C71" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>72</v>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>142</v>
       </c>
       <c r="B72" t="s">
-        <v>142</v>
-      </c>
-      <c r="C72" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>73</v>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>144</v>
       </c>
       <c r="B73" t="s">
-        <v>144</v>
-      </c>
-      <c r="C73" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>74</v>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>146</v>
       </c>
       <c r="B74" t="s">
-        <v>146</v>
-      </c>
-      <c r="C74" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>75</v>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>148</v>
       </c>
       <c r="B75" t="s">
-        <v>148</v>
-      </c>
-      <c r="C75" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>76</v>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>150</v>
       </c>
       <c r="B76" t="s">
-        <v>150</v>
-      </c>
-      <c r="C76" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>77</v>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>152</v>
       </c>
       <c r="B77" t="s">
-        <v>152</v>
-      </c>
-      <c r="C77" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>78</v>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>154</v>
       </c>
       <c r="B78" t="s">
-        <v>154</v>
-      </c>
-      <c r="C78" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>79</v>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>156</v>
       </c>
       <c r="B79" t="s">
-        <v>156</v>
-      </c>
-      <c r="C79" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>80</v>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>158</v>
       </c>
       <c r="B80" t="s">
-        <v>158</v>
-      </c>
-      <c r="C80" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>81</v>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>160</v>
       </c>
       <c r="B81" t="s">
-        <v>160</v>
-      </c>
-      <c r="C81" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>82</v>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>162</v>
       </c>
       <c r="B82" t="s">
-        <v>162</v>
-      </c>
-      <c r="C82" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>83</v>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>164</v>
       </c>
       <c r="B83" t="s">
-        <v>164</v>
-      </c>
-      <c r="C83" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>84</v>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>166</v>
       </c>
       <c r="B84" t="s">
-        <v>166</v>
-      </c>
-      <c r="C84" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>85</v>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>168</v>
       </c>
       <c r="B85" t="s">
-        <v>168</v>
-      </c>
-      <c r="C85" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>86</v>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>170</v>
       </c>
       <c r="B86" t="s">
-        <v>170</v>
-      </c>
-      <c r="C86" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>87</v>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>172</v>
       </c>
       <c r="B87" t="s">
-        <v>172</v>
-      </c>
-      <c r="C87" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>88</v>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>174</v>
       </c>
       <c r="B88" t="s">
-        <v>174</v>
-      </c>
-      <c r="C88" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>89</v>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>176</v>
       </c>
       <c r="B89" t="s">
-        <v>176</v>
-      </c>
-      <c r="C89" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>90</v>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>178</v>
       </c>
       <c r="B90" t="s">
-        <v>178</v>
-      </c>
-      <c r="C90" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>91</v>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>180</v>
       </c>
       <c r="B91" t="s">
-        <v>180</v>
-      </c>
-      <c r="C91" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>92</v>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>182</v>
       </c>
       <c r="B92" t="s">
-        <v>182</v>
-      </c>
-      <c r="C92" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>93</v>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>184</v>
       </c>
       <c r="B93" t="s">
-        <v>184</v>
-      </c>
-      <c r="C93" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>94</v>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>186</v>
       </c>
       <c r="B94" t="s">
-        <v>186</v>
-      </c>
-      <c r="C94" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>95</v>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>188</v>
       </c>
       <c r="B95" t="s">
-        <v>188</v>
-      </c>
-      <c r="C95" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>96</v>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>190</v>
       </c>
       <c r="B96" t="s">
-        <v>190</v>
-      </c>
-      <c r="C96" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>97</v>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>192</v>
       </c>
       <c r="B97" t="s">
-        <v>192</v>
-      </c>
-      <c r="C97" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>98</v>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>194</v>
       </c>
       <c r="B98" t="s">
-        <v>194</v>
-      </c>
-      <c r="C98" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>99</v>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>196</v>
       </c>
       <c r="B99" t="s">
-        <v>196</v>
-      </c>
-      <c r="C99" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>100</v>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>198</v>
       </c>
       <c r="B100" t="s">
-        <v>198</v>
-      </c>
-      <c r="C100" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>101</v>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>200</v>
       </c>
       <c r="B101" t="s">
-        <v>200</v>
-      </c>
-      <c r="C101" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102">
-        <v>102</v>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>202</v>
       </c>
       <c r="B102" t="s">
-        <v>202</v>
-      </c>
-      <c r="C102" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103">
-        <v>103</v>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>204</v>
       </c>
       <c r="B103" t="s">
-        <v>204</v>
-      </c>
-      <c r="C103" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104">
-        <v>104</v>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>206</v>
       </c>
       <c r="B104" t="s">
-        <v>206</v>
-      </c>
-      <c r="C104" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105">
-        <v>105</v>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>208</v>
       </c>
       <c r="B105" t="s">
-        <v>208</v>
-      </c>
-      <c r="C105" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106">
-        <v>106</v>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>210</v>
       </c>
       <c r="B106" t="s">
-        <v>210</v>
-      </c>
-      <c r="C106" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107">
-        <v>107</v>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>212</v>
       </c>
       <c r="B107" t="s">
-        <v>212</v>
-      </c>
-      <c r="C107" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108">
-        <v>108</v>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>214</v>
       </c>
       <c r="B108" t="s">
-        <v>214</v>
-      </c>
-      <c r="C108" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109">
-        <v>109</v>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>216</v>
       </c>
       <c r="B109" t="s">
-        <v>216</v>
-      </c>
-      <c r="C109" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110">
-        <v>110</v>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>218</v>
       </c>
       <c r="B110" t="s">
-        <v>218</v>
-      </c>
-      <c r="C110" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111">
-        <v>111</v>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>220</v>
       </c>
       <c r="B111" t="s">
-        <v>220</v>
-      </c>
-      <c r="C111" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112">
-        <v>112</v>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>222</v>
       </c>
       <c r="B112" t="s">
-        <v>222</v>
-      </c>
-      <c r="C112" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113">
-        <v>113</v>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>224</v>
       </c>
       <c r="B113" t="s">
-        <v>224</v>
-      </c>
-      <c r="C113" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114">
-        <v>114</v>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>226</v>
       </c>
       <c r="B114" t="s">
-        <v>226</v>
-      </c>
-      <c r="C114" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115">
-        <v>115</v>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>228</v>
       </c>
       <c r="B115" t="s">
-        <v>228</v>
-      </c>
-      <c r="C115" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116">
-        <v>116</v>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>230</v>
       </c>
       <c r="B116" t="s">
-        <v>230</v>
-      </c>
-      <c r="C116" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117">
-        <v>117</v>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>232</v>
       </c>
       <c r="B117" t="s">
-        <v>232</v>
-      </c>
-      <c r="C117" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118">
-        <v>118</v>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>234</v>
       </c>
       <c r="B118" t="s">
-        <v>234</v>
-      </c>
-      <c r="C118" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119">
-        <v>119</v>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>236</v>
       </c>
       <c r="B119" t="s">
-        <v>236</v>
-      </c>
-      <c r="C119" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120">
-        <v>120</v>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>238</v>
       </c>
       <c r="B120" t="s">
-        <v>238</v>
-      </c>
-      <c r="C120" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121">
-        <v>121</v>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>240</v>
       </c>
       <c r="B121" t="s">
-        <v>240</v>
-      </c>
-      <c r="C121" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122">
-        <v>122</v>
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>242</v>
       </c>
       <c r="B122" t="s">
-        <v>242</v>
-      </c>
-      <c r="C122" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123">
-        <v>123</v>
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
+        <v>244</v>
       </c>
       <c r="B123" t="s">
-        <v>244</v>
-      </c>
-      <c r="C123" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124">
-        <v>124</v>
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
+        <v>246</v>
       </c>
       <c r="B124" t="s">
-        <v>246</v>
-      </c>
-      <c r="C124" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125">
-        <v>125</v>
+    <row r="125" spans="1:2">
+      <c r="A125" t="s">
+        <v>248</v>
       </c>
       <c r="B125" t="s">
-        <v>248</v>
-      </c>
-      <c r="C125" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126">
-        <v>126</v>
+    <row r="126" spans="1:2">
+      <c r="A126" t="s">
+        <v>250</v>
       </c>
       <c r="B126" t="s">
-        <v>250</v>
-      </c>
-      <c r="C126" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127">
-        <v>127</v>
+    <row r="127" spans="1:2">
+      <c r="A127" t="s">
+        <v>252</v>
       </c>
       <c r="B127" t="s">
-        <v>252</v>
-      </c>
-      <c r="C127" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128">
-        <v>128</v>
+    <row r="128" spans="1:2">
+      <c r="A128" t="s">
+        <v>254</v>
       </c>
       <c r="B128" t="s">
-        <v>254</v>
-      </c>
-      <c r="C128" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129">
-        <v>129</v>
+    <row r="129" spans="1:2">
+      <c r="A129" t="s">
+        <v>256</v>
       </c>
       <c r="B129" t="s">
-        <v>256</v>
-      </c>
-      <c r="C129" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130">
-        <v>130</v>
+    <row r="130" spans="1:2">
+      <c r="A130" t="s">
+        <v>258</v>
       </c>
       <c r="B130" t="s">
-        <v>258</v>
-      </c>
-      <c r="C130" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131">
-        <v>131</v>
+    <row r="131" spans="1:2">
+      <c r="A131" t="s">
+        <v>260</v>
       </c>
       <c r="B131" t="s">
-        <v>260</v>
-      </c>
-      <c r="C131" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132">
-        <v>132</v>
+    <row r="132" spans="1:2">
+      <c r="A132" t="s">
+        <v>262</v>
       </c>
       <c r="B132" t="s">
-        <v>262</v>
-      </c>
-      <c r="C132" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133">
-        <v>133</v>
+    <row r="133" spans="1:2">
+      <c r="A133" t="s">
+        <v>264</v>
       </c>
       <c r="B133" t="s">
-        <v>264</v>
-      </c>
-      <c r="C133" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134">
-        <v>134</v>
+    <row r="134" spans="1:2">
+      <c r="A134" t="s">
+        <v>266</v>
       </c>
       <c r="B134" t="s">
-        <v>266</v>
-      </c>
-      <c r="C134" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135">
-        <v>135</v>
+    <row r="135" spans="1:2">
+      <c r="A135" t="s">
+        <v>268</v>
       </c>
       <c r="B135" t="s">
-        <v>268</v>
-      </c>
-      <c r="C135" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136">
-        <v>136</v>
+    <row r="136" spans="1:2">
+      <c r="A136" t="s">
+        <v>270</v>
       </c>
       <c r="B136" t="s">
-        <v>270</v>
-      </c>
-      <c r="C136" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137">
-        <v>137</v>
+    <row r="137" spans="1:2">
+      <c r="A137" t="s">
+        <v>272</v>
       </c>
       <c r="B137" t="s">
-        <v>272</v>
-      </c>
-      <c r="C137" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138">
-        <v>138</v>
+    <row r="138" spans="1:2">
+      <c r="A138" t="s">
+        <v>274</v>
       </c>
       <c r="B138" t="s">
-        <v>274</v>
-      </c>
-      <c r="C138" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139">
-        <v>139</v>
+    <row r="139" spans="1:2">
+      <c r="A139" t="s">
+        <v>276</v>
       </c>
       <c r="B139" t="s">
-        <v>276</v>
-      </c>
-      <c r="C139" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140">
-        <v>140</v>
+    <row r="140" spans="1:2">
+      <c r="A140" t="s">
+        <v>278</v>
       </c>
       <c r="B140" t="s">
-        <v>278</v>
-      </c>
-      <c r="C140" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141">
-        <v>141</v>
+    <row r="141" spans="1:2">
+      <c r="A141" t="s">
+        <v>280</v>
       </c>
       <c r="B141" t="s">
-        <v>280</v>
-      </c>
-      <c r="C141" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142">
-        <v>142</v>
+    <row r="142" spans="1:2">
+      <c r="A142" t="s">
+        <v>282</v>
       </c>
       <c r="B142" t="s">
-        <v>282</v>
-      </c>
-      <c r="C142" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143">
-        <v>143</v>
+    <row r="143" spans="1:2">
+      <c r="A143" t="s">
+        <v>284</v>
       </c>
       <c r="B143" t="s">
-        <v>284</v>
-      </c>
-      <c r="C143" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144">
-        <v>144</v>
+    <row r="144" spans="1:2">
+      <c r="A144" t="s">
+        <v>286</v>
       </c>
       <c r="B144" t="s">
-        <v>286</v>
-      </c>
-      <c r="C144" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145">
-        <v>145</v>
+    <row r="145" spans="1:2">
+      <c r="A145" t="s">
+        <v>288</v>
       </c>
       <c r="B145" t="s">
-        <v>288</v>
-      </c>
-      <c r="C145" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146">
-        <v>146</v>
+    <row r="146" spans="1:2">
+      <c r="A146" t="s">
+        <v>290</v>
       </c>
       <c r="B146" t="s">
-        <v>290</v>
-      </c>
-      <c r="C146" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147">
-        <v>147</v>
+    <row r="147" spans="1:2">
+      <c r="A147" t="s">
+        <v>292</v>
       </c>
       <c r="B147" t="s">
-        <v>292</v>
-      </c>
-      <c r="C147" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148">
-        <v>148</v>
+    <row r="148" spans="1:2">
+      <c r="A148" t="s">
+        <v>294</v>
       </c>
       <c r="B148" t="s">
-        <v>294</v>
-      </c>
-      <c r="C148" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149">
-        <v>149</v>
+    <row r="149" spans="1:2">
+      <c r="A149" t="s">
+        <v>296</v>
       </c>
       <c r="B149" t="s">
-        <v>296</v>
-      </c>
-      <c r="C149" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150">
-        <v>150</v>
+    <row r="150" spans="1:2">
+      <c r="A150" t="s">
+        <v>298</v>
       </c>
       <c r="B150" t="s">
-        <v>298</v>
-      </c>
-      <c r="C150" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151">
-        <v>151</v>
+    <row r="151" spans="1:2">
+      <c r="A151" t="s">
+        <v>300</v>
       </c>
       <c r="B151" t="s">
-        <v>300</v>
-      </c>
-      <c r="C151" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152">
-        <v>152</v>
+    <row r="152" spans="1:2">
+      <c r="A152" t="s">
+        <v>302</v>
       </c>
       <c r="B152" t="s">
-        <v>302</v>
-      </c>
-      <c r="C152" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153">
-        <v>153</v>
+    <row r="153" spans="1:2">
+      <c r="A153" t="s">
+        <v>304</v>
       </c>
       <c r="B153" t="s">
-        <v>304</v>
-      </c>
-      <c r="C153" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154">
-        <v>154</v>
+    <row r="154" spans="1:2">
+      <c r="A154" t="s">
+        <v>306</v>
       </c>
       <c r="B154" t="s">
-        <v>306</v>
-      </c>
-      <c r="C154" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155">
-        <v>155</v>
+    <row r="155" spans="1:2">
+      <c r="A155" t="s">
+        <v>308</v>
       </c>
       <c r="B155" t="s">
-        <v>308</v>
-      </c>
-      <c r="C155" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156">
-        <v>156</v>
+    <row r="156" spans="1:2">
+      <c r="A156" t="s">
+        <v>310</v>
       </c>
       <c r="B156" t="s">
-        <v>310</v>
-      </c>
-      <c r="C156" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157">
-        <v>157</v>
+    <row r="157" spans="1:2">
+      <c r="A157" t="s">
+        <v>312</v>
       </c>
       <c r="B157" t="s">
-        <v>312</v>
-      </c>
-      <c r="C157" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158">
-        <v>158</v>
+    <row r="158" spans="1:2">
+      <c r="A158" t="s">
+        <v>314</v>
       </c>
       <c r="B158" t="s">
-        <v>314</v>
-      </c>
-      <c r="C158" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159">
-        <v>159</v>
+    <row r="159" spans="1:2">
+      <c r="A159" t="s">
+        <v>316</v>
       </c>
       <c r="B159" t="s">
-        <v>316</v>
-      </c>
-      <c r="C159" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A160">
-        <v>160</v>
+    <row r="160" spans="1:2">
+      <c r="A160" t="s">
+        <v>318</v>
       </c>
       <c r="B160" t="s">
-        <v>318</v>
-      </c>
-      <c r="C160" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161">
-        <v>161</v>
+    <row r="161" spans="1:2">
+      <c r="A161" t="s">
+        <v>320</v>
       </c>
       <c r="B161" t="s">
-        <v>320</v>
-      </c>
-      <c r="C161" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162">
-        <v>162</v>
+    <row r="162" spans="1:2">
+      <c r="A162" t="s">
+        <v>322</v>
       </c>
       <c r="B162" t="s">
-        <v>322</v>
-      </c>
-      <c r="C162" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163">
-        <v>163</v>
+    <row r="163" spans="1:2">
+      <c r="A163" t="s">
+        <v>324</v>
       </c>
       <c r="B163" t="s">
-        <v>324</v>
-      </c>
-      <c r="C163" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164">
-        <v>164</v>
+    <row r="164" spans="1:2">
+      <c r="A164" t="s">
+        <v>326</v>
       </c>
       <c r="B164" t="s">
-        <v>326</v>
-      </c>
-      <c r="C164" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A165">
-        <v>165</v>
+    <row r="165" spans="1:2">
+      <c r="A165" t="s">
+        <v>328</v>
       </c>
       <c r="B165" t="s">
-        <v>328</v>
-      </c>
-      <c r="C165" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166">
-        <v>166</v>
+    <row r="166" spans="1:2">
+      <c r="A166" t="s">
+        <v>330</v>
       </c>
       <c r="B166" t="s">
-        <v>330</v>
-      </c>
-      <c r="C166" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167">
-        <v>167</v>
+    <row r="167" spans="1:2">
+      <c r="A167" t="s">
+        <v>332</v>
       </c>
       <c r="B167" t="s">
-        <v>332</v>
-      </c>
-      <c r="C167" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168">
-        <v>168</v>
+    <row r="168" spans="1:2">
+      <c r="A168" t="s">
+        <v>334</v>
       </c>
       <c r="B168" t="s">
-        <v>334</v>
-      </c>
-      <c r="C168" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169">
-        <v>169</v>
+    <row r="169" spans="1:2">
+      <c r="A169" t="s">
+        <v>336</v>
       </c>
       <c r="B169" t="s">
-        <v>336</v>
-      </c>
-      <c r="C169" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170">
-        <v>170</v>
+    <row r="170" spans="1:2">
+      <c r="A170" t="s">
+        <v>338</v>
       </c>
       <c r="B170" t="s">
-        <v>338</v>
-      </c>
-      <c r="C170" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171">
-        <v>171</v>
+    <row r="171" spans="1:2">
+      <c r="A171" t="s">
+        <v>340</v>
       </c>
       <c r="B171" t="s">
-        <v>340</v>
-      </c>
-      <c r="C171" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172">
-        <v>172</v>
+    <row r="172" spans="1:2">
+      <c r="A172" t="s">
+        <v>342</v>
       </c>
       <c r="B172" t="s">
-        <v>342</v>
-      </c>
-      <c r="C172" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173">
-        <v>173</v>
+    <row r="173" spans="1:2">
+      <c r="A173" t="s">
+        <v>344</v>
       </c>
       <c r="B173" t="s">
-        <v>344</v>
-      </c>
-      <c r="C173" t="s">
         <v>345</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>